<commit_message>
Fig. 5 of chapter options restored to match proofs
</commit_message>
<xml_diff>
--- a/Table24.5.1_AcquisitionEfficiency.xlsx
+++ b/Table24.5.1_AcquisitionEfficiency.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityhealthnetwork.sharepoint.com/teams/KamilUludagLab-BookChapterUltraHighFieldNeuroMRI/Shared Documents/BookChapterUltraHighFieldNeuroMRI/code/book-chapter-uhf-neuro-mri/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_269168717870F4850E200EC1810983A75697BD42" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC9067C4-85D3-46FF-B2A2-9687DC136955}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13560"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SummaryForFigure" sheetId="6" r:id="rId1"/>
@@ -19,17 +20,26 @@
     <definedName name="_GoBack" localSheetId="1">AllReferences!$B$10</definedName>
     <definedName name="_GoBack" localSheetId="0">SummaryForFigure!$B$7</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="111">
   <si>
     <t>Publication</t>
   </si>
@@ -319,46 +329,55 @@
     <t>bSSFP (Ehses 2018)</t>
   </si>
   <si>
-    <t>2D GRE EPI (Nasr 2016)</t>
-  </si>
-  <si>
-    <t>2D Spiral (Kasper 2022)</t>
-  </si>
-  <si>
-    <t>SMS GRE EPI (Vu 2017, HCP Pilot, R=9)</t>
-  </si>
-  <si>
-    <t>3D GRE t-Hex Spiral (Engel 2022)</t>
-  </si>
-  <si>
-    <t>3D GRE t-Hex Spiral-in (Engel 2021)</t>
-  </si>
-  <si>
     <t>Acquisition Efficiency of high-resolution UHF BOLD fMRI Sequences, computed as resolved voxels per unit time (matrix size/second)</t>
   </si>
   <si>
-    <t>2D GRE EPI (theory)</t>
-  </si>
-  <si>
-    <t>3D GRE EPI (theory)</t>
-  </si>
-  <si>
     <t>Head Gradient Specs Feinberg 2021</t>
   </si>
   <si>
-    <t>3D GRE EPI (theory, head gradient)</t>
-  </si>
-  <si>
     <t>R = 3, 6/8 Partial Fourier, at 9.4T</t>
   </si>
   <si>
     <t>(Scheffler and Ehses, 2015)</t>
+  </si>
+  <si>
+    <t>2D GE EPI (Nasr 2016)</t>
+  </si>
+  <si>
+    <t>2D GE EPI (theory)</t>
+  </si>
+  <si>
+    <t>2D GE Spiral (Kasper 2022)</t>
+  </si>
+  <si>
+    <t>3D GE EPI (Poser 2010, R=9)</t>
+  </si>
+  <si>
+    <t>SMS GE EPI (HCP 7T, R=10)</t>
+  </si>
+  <si>
+    <t>3D GE EPI (theory)</t>
+  </si>
+  <si>
+    <t>3D GE t-Hex Spiral (Engel 2022)</t>
+  </si>
+  <si>
+    <t>SMS GE EPI (Vu 2017, HCP Pilot, R=9)</t>
+  </si>
+  <si>
+    <t>3D GE EPI (van der Zwaag 2018, R=12)</t>
+  </si>
+  <si>
+    <t>3D GE t-Hex Spiral-in (Engel 2021)</t>
+  </si>
+  <si>
+    <t>3D GE EPI (theory, head gradient)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -603,6 +622,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -611,9 +633,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -674,7 +693,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -858,37 +876,37 @@
                   <c:v>bSSFP (Ehses 2018)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2D GRE EPI (Nasr 2016)</c:v>
+                  <c:v>2D GE EPI (Nasr 2016)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2D GRE EPI (theory)</c:v>
+                  <c:v>2D GE EPI (theory)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2D Spiral (Kasper 2022)</c:v>
+                  <c:v>2D GE Spiral (Kasper 2022)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3D GRE EPI (Poser 2010, R=9)</c:v>
+                  <c:v>3D GE EPI (Poser 2010, R=9)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>SMS GRE EPI (HCP 7T, R=10)</c:v>
+                  <c:v>SMS GE EPI (HCP 7T, R=10)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3D GRE EPI (theory)</c:v>
+                  <c:v>3D GE EPI (theory)</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3D GRE t-Hex Spiral (Engel 2022)</c:v>
+                  <c:v>3D GE t-Hex Spiral (Engel 2022)</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>SMS GRE EPI (Vu 2017, HCP Pilot, R=9)</c:v>
+                  <c:v>SMS GE EPI (Vu 2017, HCP Pilot, R=9)</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3D GRE EPI (van der Zwaag 2018, R=12)</c:v>
+                  <c:v>3D GE EPI (van der Zwaag 2018, R=12)</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3D GRE t-Hex Spiral-in (Engel 2021)</c:v>
+                  <c:v>3D GE t-Hex Spiral-in (Engel 2021)</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3D GRE EPI (theory, head gradient)</c:v>
+                  <c:v>3D GE EPI (theory, head gradient)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4203,7 +4221,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4240,7 +4264,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4270,7 +4300,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4550,11 +4586,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="109" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4577,22 +4613,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
+      <c r="A1" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
@@ -4604,21 +4640,21 @@
       <c r="B3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45" t="s">
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45" t="s">
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="45"/>
-      <c r="K3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="47"/>
       <c r="L3" s="41" t="s">
         <v>11</v>
       </c>
@@ -4893,7 +4929,7 @@
     </row>
     <row r="9" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>62</v>
@@ -4948,7 +4984,7 @@
     </row>
     <row r="10" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="23">
@@ -5001,7 +5037,7 @@
     </row>
     <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B11" s="39" t="s">
         <v>13</v>
@@ -5053,9 +5089,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>33</v>
@@ -5110,7 +5146,7 @@
     </row>
     <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>38</v>
@@ -5164,7 +5200,7 @@
     </row>
     <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="23">
@@ -5218,7 +5254,7 @@
     </row>
     <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>42</v>
@@ -5273,7 +5309,7 @@
     </row>
     <row r="16" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>37</v>
@@ -5327,7 +5363,7 @@
     </row>
     <row r="17" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>80</v>
@@ -5382,7 +5418,7 @@
     </row>
     <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>44</v>
@@ -5437,10 +5473,10 @@
     </row>
     <row r="19" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C19" s="23">
         <v>0.52500000000000002</v>
@@ -5508,7 +5544,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView topLeftCell="A12" zoomScale="109" workbookViewId="0">
@@ -5535,22 +5571,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
@@ -5562,21 +5598,21 @@
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45" t="s">
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45" t="s">
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="45"/>
-      <c r="K3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="47"/>
       <c r="L3" s="12" t="s">
         <v>11</v>
       </c>
@@ -6075,7 +6111,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C13" s="17">
         <v>1</v>
@@ -6122,7 +6158,7 @@
         <v>150.35761589403975</v>
       </c>
       <c r="P13" s="26" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -7379,7 +7415,7 @@
       <c r="M37" s="17"/>
     </row>
   </sheetData>
-  <sortState ref="A6:P35">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:P35">
     <sortCondition ref="O6:O35"/>
   </sortState>
   <mergeCells count="4">
@@ -7573,18 +7609,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7606,14 +7642,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AFAE056-404E-4BA6-912E-07688BB5BCC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B708C031-EBD4-49FF-AD51-1E9E481F3055}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -7627,4 +7655,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AFAE056-404E-4BA6-912E-07688BB5BCC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>